<commit_message>
Pin swap A1 and B1
Swapped to ease the routing of GND and UBD.
</commit_message>
<xml_diff>
--- a/Charger/BCU_pinout.xlsx
+++ b/Charger/BCU_pinout.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\BoatCharger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\Projekte\BoatBox\Charger\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -393,7 +393,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -799,10 +799,10 @@
   <dimension ref="D17:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="11" width="11.7109375" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
@@ -918,8 +918,8 @@
     </row>
     <row r="22" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
-      <c r="E22" s="15" t="s">
-        <v>46</v>
+      <c r="E22" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>25</v>
@@ -986,8 +986,8 @@
     </row>
     <row r="25" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D25" s="1"/>
-      <c r="E25" s="14" t="s">
-        <v>24</v>
+      <c r="E25" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>40</v>

</xml_diff>